<commit_message>
first message by D
</commit_message>
<xml_diff>
--- a/abcd.xlsx
+++ b/abcd.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52E94262-366C-4CE3-BF48-7B9B1E4F9291}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="12" yWindow="0" windowWidth="23016" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,9 +16,17 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t>dsadada</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -54,6 +63,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -100,7 +117,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -132,9 +149,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -166,6 +201,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -341,36 +394,42 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>